<commit_message>
Added Estimated Breath Cycle (EBC) sample calculations
</commit_message>
<xml_diff>
--- a/source/activity/hrv/tests/HrvAlgorithmsSampleOutput.xlsx
+++ b/source/activity/hrv/tests/HrvAlgorithmsSampleOutput.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="270" documentId="8_{9AF23D71-1F8C-4E71-814C-A0DEE8918FF2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{56D26C3E-C7CA-4001-864E-37A4782A8A65}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr showInkAnnotation="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Meditate\source\activity\hrv\tests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12150" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="RMSSD" sheetId="1" r:id="rId1"/>
     <sheet name="SDRR" sheetId="2" r:id="rId2"/>
+    <sheet name="EBC" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179016"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>bpm each second</t>
   </si>
@@ -55,12 +60,30 @@
   </si>
   <si>
     <t>SDRR 10</t>
+  </si>
+  <si>
+    <t>Max R-R (10 sec)</t>
+  </si>
+  <si>
+    <t>Min R-R (10 sec)</t>
+  </si>
+  <si>
+    <t>Max-Min R-R (10 sec)</t>
+  </si>
+  <si>
+    <t>Min R-R (16 sec)</t>
+  </si>
+  <si>
+    <t>Max R-R (16 sec)</t>
+  </si>
+  <si>
+    <t>Max-Min R-R (16 sec)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -420,22 +443,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC326162-A198-453B-8205-82D0037BE572}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0" xr3:uid="{0A361CF9-455B-5A9B-AFE9-ABA645EE46B9}">
+    <sheetView zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.9296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" customWidth="1"/>
-    <col min="3" max="3" width="22.8671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -449,7 +472,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>55</v>
       </c>
@@ -466,7 +489,7 @@
         <v>13.867504905630728</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>59</v>
       </c>
@@ -479,7 +502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>59</v>
       </c>
@@ -492,7 +515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>59</v>
       </c>
@@ -505,7 +528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>59</v>
       </c>
@@ -518,7 +541,7 @@
         <v>-33.333333333333258</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>57</v>
       </c>
@@ -531,7 +554,7 @@
         <v>16.666666666666629</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>58</v>
       </c>
@@ -544,7 +567,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>55</v>
       </c>
@@ -557,7 +580,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>58</v>
       </c>
@@ -570,7 +593,7 @@
         <v>33.333333333333371</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>60</v>
       </c>
@@ -583,7 +606,7 @@
         <v>-16.666666666666742</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>59</v>
       </c>
@@ -596,7 +619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>59</v>
       </c>
@@ -609,7 +632,7 @@
         <v>-33.333333333333258</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>57</v>
       </c>
@@ -622,7 +645,7 @@
         <v>16.666666666666629</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>58</v>
       </c>
@@ -637,28 +660,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D2FFB5-FC84-44D0-9E60-3148A46EB01E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0" xr3:uid="{8A0D323C-1588-5943-B1CC-B1B1C07F70DC}">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection sqref="A1:B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.9296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.71875" customWidth="1"/>
-    <col min="3" max="3" width="17.890625" customWidth="1"/>
-    <col min="4" max="4" width="21.92578125" customWidth="1"/>
-    <col min="5" max="5" width="14.2578125" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
     <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.953125" customWidth="1"/>
-    <col min="9" max="9" width="16.6796875" customWidth="1"/>
-    <col min="10" max="10" width="9.953125" customWidth="1"/>
-    <col min="11" max="11" width="28.78515625" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="11" max="11" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -693,7 +716,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>55</v>
       </c>
@@ -737,7 +760,7 @@
         <v>72.437038727022042</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>60</v>
       </c>
@@ -757,7 +780,7 @@
         <v>4283.55259899476</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>59</v>
       </c>
@@ -777,7 +800,7 @@
         <v>4283.55259899476</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>58</v>
       </c>
@@ -797,7 +820,7 @@
         <v>47350.628300513941</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>59</v>
       </c>
@@ -817,7 +840,7 @@
         <v>4283.55259899476</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>57</v>
       </c>
@@ -837,12 +860,12 @@
         <v>886.04010689133884</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>58</v>
       </c>
       <c r="B8">
-        <f t="shared" ref="B3:B17" si="0">(60 * 1000) / A8</f>
+        <f t="shared" ref="B8:B17" si="0">(60 * 1000) / A8</f>
         <v>1034.4827586206898</v>
       </c>
       <c r="D8">
@@ -854,7 +877,7 @@
         <v>957.50050752453058</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>55</v>
       </c>
@@ -871,7 +894,7 @@
         <v>649.37448180149283</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>58</v>
       </c>
@@ -888,7 +911,7 @@
         <v>957.50050752453058</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>60</v>
       </c>
@@ -905,7 +928,7 @@
         <v>4280.5959837109149</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>59</v>
       </c>
@@ -918,7 +941,7 @@
         <v>712.77573592896681</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>59</v>
       </c>
@@ -931,7 +954,7 @@
         <v>712.77573592896681</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>57</v>
       </c>
@@ -944,7 +967,7 @@
         <v>80.722431012508281</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>58</v>
       </c>
@@ -957,7 +980,7 @@
         <v>83.983552463813126</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>60</v>
       </c>
@@ -970,7 +993,7 @@
         <v>1905.0617158891714</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>65</v>
       </c>
@@ -981,6 +1004,224 @@
       <c r="D17">
         <f>POWER(B17 - C2, 2)</f>
         <v>14537.146506897006</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>58</v>
+      </c>
+      <c r="B2">
+        <f>(60 * 1000) / A2</f>
+        <v>1034.4827586206898</v>
+      </c>
+      <c r="C2">
+        <f>MIN(B2:B11)</f>
+        <v>1000</v>
+      </c>
+      <c r="D2">
+        <f>MAX(B2:B11)</f>
+        <v>1034.4827586206898</v>
+      </c>
+      <c r="E2">
+        <f>D2-C2</f>
+        <v>34.482758620689765</v>
+      </c>
+      <c r="F2">
+        <f>MIN(B2:B17)</f>
+        <v>1000</v>
+      </c>
+      <c r="G2">
+        <f>MAX(B2:B17)</f>
+        <v>1052.6315789473683</v>
+      </c>
+      <c r="H2">
+        <f>G2-F2</f>
+        <v>52.631578947368325</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>60</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B17" si="0">(60 * 1000) / A3</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>59</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>1016.9491525423729</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>58</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>1034.4827586206898</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>59</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>1016.9491525423729</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>58</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>1034.4827586206898</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>58</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>1034.4827586206898</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>59</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>1016.9491525423729</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>58</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>1034.4827586206898</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>60</v>
+      </c>
+      <c r="B11">
+        <f>(60 * 1000) / A11</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>60</v>
+      </c>
+      <c r="B12">
+        <f>(60 * 1000) / A12</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>59</v>
+      </c>
+      <c r="B13">
+        <f>(60 * 1000) / A13</f>
+        <v>1016.9491525423729</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>59</v>
+      </c>
+      <c r="B14">
+        <f>(60 * 1000) / A14</f>
+        <v>1016.9491525423729</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>57</v>
+      </c>
+      <c r="B15">
+        <f>(60 * 1000) / A15</f>
+        <v>1052.6315789473683</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>58</v>
+      </c>
+      <c r="B16">
+        <f>(60 * 1000) / A16</f>
+        <v>1034.4827586206898</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>60</v>
+      </c>
+      <c r="B17">
+        <f>(60 * 1000) / A17</f>
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added HRV Estimated Breath Cycle for 10 and 16 intervals continuous monitoring in data field chart
</commit_message>
<xml_diff>
--- a/source/activity/hrv/tests/HrvAlgorithmsSampleOutput.xlsx
+++ b/source/activity/hrv/tests/HrvAlgorithmsSampleOutput.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr showInkAnnotation="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Meditate\source\activity\hrv\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_3DC74F0148C77A779BAB0A7D334CF5B224FEA57C" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{43460DD9-5724-439F-B3F4-CABB52E11748}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12150" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12150" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RMSSD" sheetId="1" r:id="rId1"/>
     <sheet name="SDRR" sheetId="2" r:id="rId2"/>
     <sheet name="EBC" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179016"/>
 </workbook>
 </file>
 
@@ -83,7 +84,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -443,22 +444,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.64453125" customWidth="1"/>
+    <col min="3" max="3" width="22.8671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,7 +473,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>55</v>
       </c>
@@ -489,7 +490,7 @@
         <v>13.867504905630728</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>59</v>
       </c>
@@ -502,7 +503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>59</v>
       </c>
@@ -515,7 +516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>59</v>
       </c>
@@ -528,7 +529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>59</v>
       </c>
@@ -541,7 +542,7 @@
         <v>-33.333333333333258</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>57</v>
       </c>
@@ -554,7 +555,7 @@
         <v>16.666666666666629</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>58</v>
       </c>
@@ -567,7 +568,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>55</v>
       </c>
@@ -580,7 +581,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>58</v>
       </c>
@@ -593,7 +594,7 @@
         <v>33.333333333333371</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>60</v>
       </c>
@@ -606,7 +607,7 @@
         <v>-16.666666666666742</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>59</v>
       </c>
@@ -619,7 +620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>59</v>
       </c>
@@ -632,7 +633,7 @@
         <v>-33.333333333333258</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>57</v>
       </c>
@@ -645,7 +646,7 @@
         <v>16.666666666666629</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>58</v>
       </c>
@@ -660,28 +661,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
       <selection sqref="A1:B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.37109375" customWidth="1"/>
+    <col min="2" max="2" width="13.71875" customWidth="1"/>
+    <col min="3" max="3" width="17.890625" customWidth="1"/>
+    <col min="4" max="4" width="21.7890625" customWidth="1"/>
+    <col min="5" max="5" width="14.2578125" customWidth="1"/>
     <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" customWidth="1"/>
-    <col min="10" max="10" width="10" customWidth="1"/>
-    <col min="11" max="11" width="28.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9.953125" customWidth="1"/>
+    <col min="9" max="9" width="16.6796875" customWidth="1"/>
+    <col min="10" max="10" width="9.953125" customWidth="1"/>
+    <col min="11" max="11" width="28.65234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -716,7 +717,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>55</v>
       </c>
@@ -760,7 +761,7 @@
         <v>72.437038727022042</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>60</v>
       </c>
@@ -780,7 +781,7 @@
         <v>4283.55259899476</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>59</v>
       </c>
@@ -800,7 +801,7 @@
         <v>4283.55259899476</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>58</v>
       </c>
@@ -820,7 +821,7 @@
         <v>47350.628300513941</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>59</v>
       </c>
@@ -840,7 +841,7 @@
         <v>4283.55259899476</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>57</v>
       </c>
@@ -860,7 +861,7 @@
         <v>886.04010689133884</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>58</v>
       </c>
@@ -877,7 +878,7 @@
         <v>957.50050752453058</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>55</v>
       </c>
@@ -894,7 +895,7 @@
         <v>649.37448180149283</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>58</v>
       </c>
@@ -911,7 +912,7 @@
         <v>957.50050752453058</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>60</v>
       </c>
@@ -928,7 +929,7 @@
         <v>4280.5959837109149</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>59</v>
       </c>
@@ -941,7 +942,7 @@
         <v>712.77573592896681</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>59</v>
       </c>
@@ -954,7 +955,7 @@
         <v>712.77573592896681</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>57</v>
       </c>
@@ -967,7 +968,7 @@
         <v>80.722431012508281</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>58</v>
       </c>
@@ -980,7 +981,7 @@
         <v>83.983552463813126</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>60</v>
       </c>
@@ -993,7 +994,7 @@
         <v>1905.0617158891714</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>65</v>
       </c>
@@ -1012,25 +1013,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.23828125" customWidth="1"/>
+    <col min="3" max="3" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.46875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.46875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.25390625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1056,7 +1058,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>58</v>
       </c>
@@ -1065,19 +1067,19 @@
         <v>1034.4827586206898</v>
       </c>
       <c r="C2">
-        <f>MIN(B2:B11)</f>
+        <f>MIN(J2:J11)</f>
         <v>1000</v>
       </c>
       <c r="D2">
-        <f>MAX(B2:B11)</f>
-        <v>1034.4827586206898</v>
+        <f>MAX(J2:J11)</f>
+        <v>1034.48</v>
       </c>
       <c r="E2">
         <f>D2-C2</f>
-        <v>34.482758620689765</v>
+        <v>34.480000000000018</v>
       </c>
       <c r="F2">
-        <f>MIN(B2:B17)</f>
+        <f>MIN(J2:J17)</f>
         <v>1000</v>
       </c>
       <c r="G2">
@@ -1088,8 +1090,11 @@
         <f>G2-F2</f>
         <v>52.631578947368325</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>1034.48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>60</v>
       </c>
@@ -1097,8 +1102,11 @@
         <f t="shared" ref="B3:B17" si="0">(60 * 1000) / A3</f>
         <v>1000</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>59</v>
       </c>
@@ -1106,8 +1114,11 @@
         <f t="shared" si="0"/>
         <v>1016.9491525423729</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>1016.94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>58</v>
       </c>
@@ -1115,8 +1126,11 @@
         <f t="shared" si="0"/>
         <v>1034.4827586206898</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>1034.48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>59</v>
       </c>
@@ -1124,8 +1138,11 @@
         <f t="shared" si="0"/>
         <v>1016.9491525423729</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>1016.94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>58</v>
       </c>
@@ -1133,8 +1150,11 @@
         <f t="shared" si="0"/>
         <v>1034.4827586206898</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>1034.48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>58</v>
       </c>
@@ -1142,8 +1162,11 @@
         <f t="shared" si="0"/>
         <v>1034.4827586206898</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>1034.48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>59</v>
       </c>
@@ -1151,8 +1174,11 @@
         <f t="shared" si="0"/>
         <v>1016.9491525423729</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>1016.94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>58</v>
       </c>
@@ -1160,8 +1186,11 @@
         <f t="shared" si="0"/>
         <v>1034.4827586206898</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>1034.48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>60</v>
       </c>
@@ -1169,8 +1198,11 @@
         <f>(60 * 1000) / A11</f>
         <v>1000</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>60</v>
       </c>
@@ -1178,8 +1210,11 @@
         <f>(60 * 1000) / A12</f>
         <v>1000</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>59</v>
       </c>
@@ -1187,8 +1222,11 @@
         <f>(60 * 1000) / A13</f>
         <v>1016.9491525423729</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>1016.94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>59</v>
       </c>
@@ -1196,8 +1234,11 @@
         <f>(60 * 1000) / A14</f>
         <v>1016.9491525423729</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>1016.94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>57</v>
       </c>
@@ -1205,8 +1246,11 @@
         <f>(60 * 1000) / A15</f>
         <v>1052.6315789473683</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>1052.6300000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>58</v>
       </c>
@@ -1214,13 +1258,19 @@
         <f>(60 * 1000) / A16</f>
         <v>1034.4827586206898</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <v>1034.48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>60</v>
       </c>
       <c r="B17">
         <f>(60 * 1000) / A17</f>
+        <v>1000</v>
+      </c>
+      <c r="J17">
         <v>1000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Max-Min HR Window Stress stats calculator
</commit_message>
<xml_diff>
--- a/source/activity/hrv/tests/HrvAlgorithmsSampleOutput.xlsx
+++ b/source/activity/hrv/tests/HrvAlgorithmsSampleOutput.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Meditate\source\activity\hrv\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_3DC74F0148C77A779BAB0A7D334CF5B224FEA57C" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{43460DD9-5724-439F-B3F4-CABB52E11748}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="11_3DC74F0148C77A779BAB0A7D334CF5B224FEA57C" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{0B25F5F9-7E13-415F-803E-F5650B425DE5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12150" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12150" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RMSSD" sheetId="1" r:id="rId1"/>
     <sheet name="SDRR" sheetId="2" r:id="rId2"/>
     <sheet name="EBC" sheetId="3" r:id="rId3"/>
+    <sheet name="Max-Min HR Window 10 Sec Stats" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179016"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>bpm each second</t>
   </si>
@@ -79,6 +80,24 @@
   </si>
   <si>
     <t>Max-Min R-R (16 sec)</t>
+  </si>
+  <si>
+    <t>Max-Min HR Window Calculation</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>No Stress</t>
+  </si>
+  <si>
+    <t>Medium Stress</t>
+  </si>
+  <si>
+    <t>High Stress</t>
+  </si>
+  <si>
+    <t>Max-Min HR Window Calculation Filtered Outliers</t>
   </si>
 </sst>
 </file>
@@ -1016,7 +1035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
+    <sheetView workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1277,4 +1296,318 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8375A381-6568-403D-B16E-684F7936B506}">
+  <dimension ref="A1:H26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0" xr3:uid="{F34976B4-FE0C-5677-BE68-F6B0D0F4DDB3}">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.2265625" customWidth="1"/>
+    <col min="3" max="3" width="13.31640625" customWidth="1"/>
+    <col min="4" max="4" width="10.22265625" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.76171875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <f>IF(A2&lt;10, A2, 10)</f>
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <f>MEDIAN(B2:B26)</f>
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <f>COUNTIF(B2:B26, "&lt;="&amp;C2)/COUNT(B2:B26)</f>
+        <v>0.52</v>
+      </c>
+      <c r="E2">
+        <f>COUNTIF(B2:B26, "&gt;"&amp;C2)/COUNT(B2:B26)-F2</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="F2">
+        <f>COUNTIF(B2:B26, "&gt;=10")/COUNT(B2:B26)</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B26" si="0">IF(A3&lt;10, A3, 10)</f>
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>6</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>7</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added more test cases and fixes for MaxMinHrWindowStats; exposed the data as summary fit fields and on the summary screen
</commit_message>
<xml_diff>
--- a/source/activity/hrv/tests/HrvAlgorithmsSampleOutput.xlsx
+++ b/source/activity/hrv/tests/HrvAlgorithmsSampleOutput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Meditate\source\activity\hrv\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="133" documentId="11_3DC74F0148C77A779BAB0A7D334CF5B224FEA57C" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{0B25F5F9-7E13-415F-803E-F5650B425DE5}"/>
+  <xr:revisionPtr revIDLastSave="226" documentId="11_3DC74F0148C77A779BAB0A7D334CF5B224FEA57C" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{1321353A-862B-44A8-9F07-A9BE4E877EFC}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12150" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -146,9 +146,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1300,10 +1301,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8375A381-6568-403D-B16E-684F7936B506}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0" xr3:uid="{F34976B4-FE0C-5677-BE68-F6B0D0F4DDB3}">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1316,7 +1317,7 @@
     <col min="6" max="6" width="10.76171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -1335,84 +1336,98 @@
       <c r="F1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <f>IF(A2&lt;10, A2, 10)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <f>MEDIAN(B2:B26)</f>
-        <v>6</v>
+        <f>MEDIAN(B2:B11)</f>
+        <v>4.5</v>
       </c>
       <c r="D2">
-        <f>COUNTIF(B2:B26, "&lt;="&amp;C2)/COUNT(B2:B26)</f>
-        <v>0.52</v>
+        <f>COUNTIF(B2:B11, "&lt;="&amp;C2)/COUNT(B2:B11)</f>
+        <v>0.5</v>
       </c>
       <c r="E2">
-        <f>COUNTIF(B2:B26, "&gt;"&amp;C2)/COUNT(B2:B26)-F2</f>
-        <v>0.19999999999999996</v>
+        <f>COUNTIF(B2:B11, "&gt;"&amp;C2)/COUNT(B2:B11)-F2</f>
+        <v>0.5</v>
       </c>
       <c r="F2">
-        <f>COUNTIF(B2:B26, "&gt;=10")/COUNT(B2:B26)</f>
-        <v>0.28000000000000003</v>
+        <f>COUNTIF(B2:B11, "&gt;=10")/COUNT(B2:B11)</f>
+        <v>0</v>
       </c>
       <c r="H2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <f>MEDIAN(I1:I20)</f>
+        <v>10</v>
+      </c>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B26" si="0">IF(A3&lt;10, A3, 10)</f>
-        <v>4</v>
+        <f>IF(A3&lt;10, A3, 10)</f>
+        <v>1</v>
       </c>
       <c r="H3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B3:B26" si="0">IF(A4&lt;10, A4, 10)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="B7">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>13</v>
-      </c>
-      <c r="B6">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>12</v>
-      </c>
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1421,7 +1436,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1430,37 +1445,37 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H12">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>13</v>
       </c>
@@ -1472,7 +1487,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1484,7 +1499,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>6</v>
       </c>
@@ -1496,7 +1511,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Extracted StressMonitor out of HrvMonitor and split the depedent classes and unit tests; removed EBC tracking; added global settings for configuring Stress Tracking and HRV tracking
</commit_message>
<xml_diff>
--- a/source/activity/hrv/tests/HrvAlgorithmsSampleOutput.xlsx
+++ b/source/activity/hrv/tests/HrvAlgorithmsSampleOutput.xlsx
@@ -8,22 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Meditate\source\activity\hrv\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="226" documentId="11_3DC74F0148C77A779BAB0A7D334CF5B224FEA57C" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{1321353A-862B-44A8-9F07-A9BE4E877EFC}"/>
+  <xr:revisionPtr revIDLastSave="256" documentId="11_3DC74F0148C77A779BAB0A7D334CF5B224FEA57C" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{BC96DE4D-F00F-4314-8802-C0CC26D1BAB8}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12150" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12150" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RMSSD" sheetId="1" r:id="rId1"/>
     <sheet name="SDRR" sheetId="2" r:id="rId2"/>
     <sheet name="EBC" sheetId="3" r:id="rId3"/>
-    <sheet name="Max-Min HR Window 10 Sec Stats" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179016"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>bpm each second</t>
   </si>
@@ -80,24 +79,6 @@
   </si>
   <si>
     <t>Max-Min R-R (16 sec)</t>
-  </si>
-  <si>
-    <t>Max-Min HR Window Calculation</t>
-  </si>
-  <si>
-    <t>Median</t>
-  </si>
-  <si>
-    <t>No Stress</t>
-  </si>
-  <si>
-    <t>Medium Stress</t>
-  </si>
-  <si>
-    <t>High Stress</t>
-  </si>
-  <si>
-    <t>Max-Min HR Window Calculation Filtered Outliers</t>
   </si>
 </sst>
 </file>
@@ -146,10 +127,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -476,7 +456,7 @@
     <col min="1" max="1" width="14.9296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.64453125" customWidth="1"/>
     <col min="3" max="3" width="22.8671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5859375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1036,12 +1016,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="17.3515625" customWidth="1"/>
     <col min="2" max="2" width="12.23828125" customWidth="1"/>
     <col min="3" max="3" width="15.19921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.46875" bestFit="1" customWidth="1"/>
@@ -1297,332 +1278,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8375A381-6568-403D-B16E-684F7936B506}">
-  <dimension ref="A1:K26"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0" xr3:uid="{F34976B4-FE0C-5677-BE68-F6B0D0F4DDB3}">
-      <selection activeCell="I6" sqref="I6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="27.84375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.2265625" customWidth="1"/>
-    <col min="3" max="3" width="13.31640625" customWidth="1"/>
-    <col min="4" max="4" width="10.22265625" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.76171875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <f>IF(A2&lt;10, A2, 10)</f>
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <f>MEDIAN(B2:B11)</f>
-        <v>4.5</v>
-      </c>
-      <c r="D2">
-        <f>COUNTIF(B2:B11, "&lt;="&amp;C2)/COUNT(B2:B11)</f>
-        <v>0.5</v>
-      </c>
-      <c r="E2">
-        <f>COUNTIF(B2:B11, "&gt;"&amp;C2)/COUNT(B2:B11)-F2</f>
-        <v>0.5</v>
-      </c>
-      <c r="F2">
-        <f>COUNTIF(B2:B11, "&gt;=10")/COUNT(B2:B11)</f>
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
-      <c r="I2">
-        <v>10</v>
-      </c>
-      <c r="J2">
-        <f>MEDIAN(I1:I20)</f>
-        <v>10</v>
-      </c>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <f>IF(A3&lt;10, A3, 10)</f>
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <f t="shared" ref="B3:B26" si="0">IF(A4&lt;10, A4, 10)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="H12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>13</v>
-      </c>
-      <c r="B13">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="H13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="H14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>6</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="H15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>7</v>
-      </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="H16">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>3</v>
-      </c>
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H17">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>7</v>
-      </c>
-      <c r="B18">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="H18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>2</v>
-      </c>
-      <c r="B19">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>3</v>
-      </c>
-      <c r="B20">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>17</v>
-      </c>
-      <c r="B21">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>25</v>
-      </c>
-      <c r="B23">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>8</v>
-      </c>
-      <c r="B24">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>3</v>
-      </c>
-      <c r="B25">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>4</v>
-      </c>
-      <c r="B26">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>